<commit_message>
Use 6.9% DM not 5.1% for digestate
</commit_message>
<xml_diff>
--- a/2021-0294105_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_NH3_EFs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Slurry" sheetId="1" state="visible" r:id="rId2"/>
@@ -292,8 +292,8 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,7 +353,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>5.1</v>
+        <v>6.9</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>7.9</v>
@@ -397,7 +397,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>5.1</v>
+        <v>6.9</v>
       </c>
       <c r="D7" s="4" t="n">
         <f aca="false">D4-1.38</f>
@@ -422,7 +422,7 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Switch to digestate 5.9% DM n =26
</commit_message>
<xml_diff>
--- a/2021-0294105_NH3_EFs/inputs/inputs.xlsx
+++ b/2021-0294105_NH3_EFs/inputs/inputs.xlsx
@@ -293,7 +293,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,7 +353,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>7.9</v>
@@ -397,7 +397,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="D7" s="4" t="n">
         <f aca="false">D4-1.38</f>

</xml_diff>